<commit_message>
each question answer tracked
</commit_message>
<xml_diff>
--- a/quiz-questions.xlsx
+++ b/quiz-questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\enneagram-quiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9BFA52-1C36-418F-A55D-2FCB2374D4F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48DF671-9AC7-4D3E-AFE0-F64038D5DF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,144 +47,142 @@
     <t>Targets Type 1's core motivation for integrity and fear of being corrupt or wrong. This question helps highlight the inner critic and the striving for moral high ground.</t>
   </si>
   <si>
+    <t>"I find it difficult to relax when I see something that needs improvement or fixing."</t>
+  </si>
+  <si>
+    <t>"I feel strongly that fairness and justice should be upheld as a matter of principle."</t>
+  </si>
+  <si>
+    <t>"I often feel a moral obligation to meet higher standards than I expect from others."</t>
+  </si>
+  <si>
+    <t>Further captures Type 1's commitment to ethics and their discomfort with perceived injustices or unfairness.</t>
+  </si>
+  <si>
+    <t>Reflects Type 1’s perfectionism and internal self-criticism. This explores their inner drive for improvement.</t>
+  </si>
+  <si>
+    <t>"I feel unsettled when things don’t meet my standards of order and correctness."</t>
+  </si>
+  <si>
+    <t>Highlights Type 1's focus on structure and aversion to chaos.</t>
+  </si>
+  <si>
+    <t>"I believe that rules, structure, and doing what’s right are essential for creating a better world."</t>
+  </si>
+  <si>
+    <t>Addresses Type 1’s adherence to principles and their tendency to see the world in terms of right and wrong.</t>
+  </si>
+  <si>
+    <t>"I feel frustrated when things or people don’t live up to the standards I hold."</t>
+  </si>
+  <si>
+    <t>"I often neglect my own needs because I feel fulfilled when I’m making others feel loved and supported."</t>
+  </si>
+  <si>
+    <t>Explores Type 2’s core motivation to be loved and valued through helpfulness and connection. This emphasizes their tendency to derive self-worth from being indispensable.</t>
+  </si>
+  <si>
+    <t>"I feel happiest when I’m making someone else’s life easier or better, and it's appreciated."</t>
+  </si>
+  <si>
+    <t>Reflects Type 2’s joy in serving others and their need for connection and appreciation.</t>
+  </si>
+  <si>
+    <t>"I sometimes feel hurt if my efforts to help others are not acknowledged."</t>
+  </si>
+  <si>
+    <t>Captures Type 2’s vulnerability to feeling unappreciated and their need for validation.</t>
+  </si>
+  <si>
+    <t>"I often anticipate others’ needs before they even ask for help."</t>
+  </si>
+  <si>
+    <t>Highlights Type 2’s focus on intuitively understanding and meeting the needs of others.</t>
+  </si>
+  <si>
+    <t>"I instinctively notice when someone needs support and feel drawn to help them."</t>
+  </si>
+  <si>
+    <t>"I feel a strong emotional need to be needed and valued by the people I care about."</t>
+  </si>
+  <si>
     <t>Addresses Type 2’s motivation to feel indispensable and appreciated.</t>
   </si>
   <si>
+    <t>"I feel driven to succeed and fear being seen as a failure or incapable."</t>
+  </si>
+  <si>
     <t>Highlights Type 3's drive for achievement and fear of being seen as unworthy. It touches on the pressure they feel to excel and prove their value.</t>
   </si>
   <si>
+    <t>"I often adjust my personality or behavior to match the expectations of others."</t>
+  </si>
+  <si>
+    <t>Reflects Type 3’s adaptability and their focus on achieving recognition through alignment with others’ values.</t>
+  </si>
+  <si>
+    <t>"I naturally detect what others value and scan for opportunities to shine and advance."</t>
+  </si>
+  <si>
+    <t>Addresses Type 3’s drive to excel and their fear of being seen as average or unremarkable.</t>
+  </si>
+  <si>
+    <t>"I feel restless and unsatisfied if I’m not actively working toward something significant, or an ambitious goal."</t>
+  </si>
+  <si>
+    <t>Highlights Type 3’s focus on image and external validation.</t>
+  </si>
+  <si>
+    <t>"I measure my worth by how much I’m able to achieve."</t>
+  </si>
+  <si>
+    <t>Captures Type 3’s core motivation and their focus on results and accomplishment.</t>
+  </si>
+  <si>
+    <t>"I feel a strong sense of purpose when I’m being recognized for what I accomplish."</t>
+  </si>
+  <si>
+    <t>"I feel most alive when I’m expressing something that reflects my unique identity and emotional depth."</t>
+  </si>
+  <si>
+    <t>Probes Type 4’s introspection and longing to find a unique identity. This helps identify their depth of emotion and their search for significance.</t>
+  </si>
+  <si>
+    <t>"I sometimes feel like I don’t fully belong, as if there’s something missing or different about me."</t>
+  </si>
+  <si>
+    <t>Reflects Type 4’s tendency to feel different and their yearning for a place where they are truly understood.</t>
+  </si>
+  <si>
+    <t>"I find beauty and meaning in experiences that others might overlook as ordinary."</t>
+  </si>
+  <si>
+    <t>Highlights Type 4’s focus on emotional richness and their ability to see value in subtlety and creativity.</t>
+  </si>
+  <si>
+    <t>"I often feel a longing for something that is difficult to define."</t>
+  </si>
+  <si>
+    <t>Captures Type 4’s core emotional focus on yearning and searching for meaning.</t>
+  </si>
+  <si>
+    <t>"I dislike the idea of blending in with the crowd and look for ways to express my individuality."</t>
+  </si>
+  <si>
     <t>Addresses Type 4’s desire to stand out and their resistance to being perceived as ordinary.</t>
   </si>
   <si>
+    <t>"I’m drawn to exploring and understanding the deeper emotional truths behind my experiences."</t>
+  </si>
+  <si>
     <t>"I feel the need to gather as much knowledge as I can before making decisions."</t>
   </si>
   <si>
     <t>Reflects Type 5’s need for understanding and fear of being helpless or incapable. This explores their analytical nature and self-reliance.</t>
   </si>
   <si>
-    <t>"I find it difficult to relax when I see something that needs improvement or fixing."</t>
-  </si>
-  <si>
-    <t>"I feel strongly that fairness and justice should be upheld as a matter of principle."</t>
-  </si>
-  <si>
-    <t>Further captures Type 1's commitment to ethics and their discomfort with perceived injustices or unfairness.</t>
-  </si>
-  <si>
-    <t>"I often feel a moral obligation to meet higher standards than I expect from others."</t>
-  </si>
-  <si>
-    <t>Reflects Type 1’s perfectionism and internal self-criticism. This explores their inner drive for improvement.</t>
-  </si>
-  <si>
-    <t>"I feel unsettled when things don’t meet my standards of order and correctness."</t>
-  </si>
-  <si>
-    <t>Highlights Type 1's focus on structure and aversion to chaos.</t>
-  </si>
-  <si>
-    <t>"I believe that rules, structure, and doing what’s right are essential for creating a better world."</t>
-  </si>
-  <si>
-    <t>Addresses Type 1’s adherence to principles and their tendency to see the world in terms of right and wrong.</t>
-  </si>
-  <si>
-    <t>"I feel frustrated when things or people don’t live up to the standards I hold."</t>
-  </si>
-  <si>
-    <t>"I often neglect my own needs because I feel fulfilled when I’m making others feel loved and supported."</t>
-  </si>
-  <si>
-    <t>Explores Type 2’s core motivation to be loved and valued through helpfulness and connection. This emphasizes their tendency to derive self-worth from being indispensable.</t>
-  </si>
-  <si>
-    <t>"I feel happiest when I’m making someone else’s life easier or better, and it's appreciated."</t>
-  </si>
-  <si>
-    <t>Reflects Type 2’s joy in serving others and their need for connection and appreciation.</t>
-  </si>
-  <si>
-    <t>"I sometimes feel hurt if my efforts to help others are not acknowledged."</t>
-  </si>
-  <si>
-    <t>Captures Type 2’s vulnerability to feeling unappreciated and their need for validation.</t>
-  </si>
-  <si>
-    <t>"I often anticipate others’ needs before they even ask for help."</t>
-  </si>
-  <si>
-    <t>Highlights Type 2’s focus on intuitively understanding and meeting the needs of others.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"I instinctively notice when someone needs support and feel drawn to help them."
-</t>
-  </si>
-  <si>
-    <t>"I feel a strong emotional need to be needed and valued by the people I care about."</t>
-  </si>
-  <si>
-    <t>"I feel driven to succeed and fear being seen as a failure or incapable."</t>
-  </si>
-  <si>
-    <t>"I often adjust my personality or behavior to match the expectations of others."</t>
-  </si>
-  <si>
-    <t>Reflects Type 3’s adaptability and their focus on achieving recognition through alignment with others’ values.</t>
-  </si>
-  <si>
-    <t>"I naturally detect what others value and scan for opportunities to shine and advance."</t>
-  </si>
-  <si>
-    <t>Addresses Type 3’s drive to excel and their fear of being seen as average or unremarkable.</t>
-  </si>
-  <si>
-    <t>"I feel restless and unsatisfied if I’m not actively working toward something significant, or an ambitious goal."</t>
-  </si>
-  <si>
-    <t>Highlights Type 3’s focus on image and external validation.</t>
-  </si>
-  <si>
-    <t>"I measure my worth by how much I’m able to achieve."</t>
-  </si>
-  <si>
-    <t>Captures Type 3’s core motivation and their focus on results and accomplishment.</t>
-  </si>
-  <si>
-    <t>"I feel a strong sense of purpose when I’m being recognized for what I accomplish."</t>
-  </si>
-  <si>
-    <t>"I feel most alive when I’m expressing something that reflects my unique identity and emotional depth."</t>
-  </si>
-  <si>
-    <t>Probes Type 4’s introspection and longing to find a unique identity. This helps identify their depth of emotion and their search for significance.</t>
-  </si>
-  <si>
-    <t>"I sometimes feel like I don’t fully belong, as if there’s something missing or different about me."</t>
-  </si>
-  <si>
-    <t>Reflects Type 4’s tendency to feel different and their yearning for a place where they are truly understood.</t>
-  </si>
-  <si>
-    <t>"I find beauty and meaning in experiences that others might overlook as ordinary."</t>
-  </si>
-  <si>
-    <t>Highlights Type 4’s focus on emotional richness and their ability to see value in subtlety and creativity.</t>
-  </si>
-  <si>
-    <t>"I often feel a longing for something that is difficult to define."</t>
-  </si>
-  <si>
-    <t>Captures Type 4’s core emotional focus on yearning and searching for meaning.</t>
-  </si>
-  <si>
-    <t>"I dislike the idea of blending in with the crowd and look for ways to express my individuality."</t>
-  </si>
-  <si>
-    <t>"I’m drawn to exploring and understanding the deeper emotional truths behind my experiences."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"I feel most at ease when I have the space to handle things on my own."
-</t>
+    <t>"I feel most at ease when I have the space to handle things on my own."</t>
   </si>
   <si>
     <t>Highlights Type 5’s focus on autonomy and their discomfort with excessive reliance on external support.</t>
@@ -340,8 +338,7 @@
     <t>Captures Type 9’s desire for unity and their aversion to discord.</t>
   </si>
   <si>
-    <t xml:space="preserve">"I feel most at ease when everyone around me is getting along and there’s no tension."
-</t>
+    <t>"I feel most at ease when everyone around me is getting along and there’s no tension."</t>
   </si>
 </sst>
 </file>
@@ -731,20 +728,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="68.21875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="1" width="121.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -760,9 +757,9 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="119.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -772,160 +769,151 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
       </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="4">
         <v>1</v>
       </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5">
         <v>2</v>
       </c>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C9" s="5">
         <v>2</v>
       </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C10" s="5">
         <v>2</v>
       </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C11" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C13" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C14" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C15" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C16" s="6">
         <v>3</v>
@@ -933,10 +921,10 @@
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C17" s="6">
         <v>3</v>
@@ -944,10 +932,10 @@
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C18" s="6">
         <v>3</v>
@@ -955,7 +943,7 @@
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="6">
@@ -964,10 +952,10 @@
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C20" s="7">
         <v>4</v>
@@ -975,10 +963,10 @@
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C21" s="7">
         <v>4</v>
@@ -986,10 +974,10 @@
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C22" s="7">
         <v>4</v>
@@ -997,10 +985,10 @@
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C23" s="7">
         <v>4</v>
@@ -1008,10 +996,10 @@
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C24" s="7">
         <v>4</v>
@@ -1019,7 +1007,7 @@
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="7">
@@ -1028,10 +1016,10 @@
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="C26" s="8">
         <v>5</v>

</xml_diff>